<commit_message>
inspection on data files and made cij just for current classes
</commit_message>
<xml_diff>
--- a/Data/derslik_20190410.xlsx
+++ b/Data/derslik_20190410.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\PycharmProjects\inputBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melda Aktepe\PycharmProjects\inputBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7928792-570A-42B1-A6E2-FBD73C179673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488F2C2D-54DB-47B7-97FB-17EE280E5A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Worksheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5365" uniqueCount="321">
   <si>
     <t>BLDG</t>
   </si>
@@ -971,6 +971,21 @@
   </si>
   <si>
     <t>VA 401;VA 402;</t>
+  </si>
+  <si>
+    <t>STUDYO</t>
+  </si>
+  <si>
+    <t>drow</t>
+  </si>
+  <si>
+    <t>drowing</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1012</t>
   </si>
 </sst>
 </file>
@@ -1010,11 +1025,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,11 +1345,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H877"/>
+  <dimension ref="A1:H879"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B878" sqref="B878:B879"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21782,6 +21798,52 @@
         <v>33</v>
       </c>
     </row>
+    <row r="878" spans="1:7">
+      <c r="A878" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B878" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C878" t="s">
+        <v>316</v>
+      </c>
+      <c r="D878" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E878" s="1">
+        <v>30</v>
+      </c>
+      <c r="F878" t="s">
+        <v>317</v>
+      </c>
+      <c r="G878" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="879" spans="1:7">
+      <c r="A879" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B879" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C879" t="s">
+        <v>316</v>
+      </c>
+      <c r="D879" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E879" s="1">
+        <v>30</v>
+      </c>
+      <c r="F879" t="s">
+        <v>317</v>
+      </c>
+      <c r="G879" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>